<commit_message>
#Que no me deje asociar la partida mas de una vez - Realizado #Que no me deje confirmar la adquisición si ya compre todo para la partida asociada - Realizado
</commit_message>
<xml_diff>
--- a/Anotaciones/Tareas.xlsx
+++ b/Anotaciones/Tareas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Que no me deje asociar la partida mas de una vez</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Traducción en las grillas</t>
+  </si>
+  <si>
+    <t>Colores en forms</t>
+  </si>
+  <si>
+    <t>Que si cancelo imprimir al crear partida, me cancele todas las impresiones</t>
   </si>
 </sst>
 </file>
@@ -53,12 +59,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -73,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,55 +392,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B10">
+    <sortCondition ref="B2:B10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#Fix Imprimir en Partida SOlicitar y Crear #Fix Caso uso Casos uso/SC001 - Crear Solicitud.docx
</commit_message>
<xml_diff>
--- a/Anotaciones/Tareas.xlsx
+++ b/Anotaciones/Tareas.xlsx
@@ -395,7 +395,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3">

</xml_diff>

<commit_message>
Que si cancelo imprimir al crear partida, me cancele todas las impresiones Agregar y quitar cotizaciones a Partidas siempre tienen que quedar tres y el estado de SolicDetalle asociado no cambia Agregar Inventarios a una Adquisición ya creada, Fix Quitar Inventarios a una Adquisicion - Fix Documentos de rendición, rutas, idioma e imprimir Documentos de Asignacion, rutas, idioma e imprimir
#Traducción en MBox de Backup
</commit_message>
<xml_diff>
--- a/Anotaciones/Tareas.xlsx
+++ b/Anotaciones/Tareas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Que no me deje asociar la partida mas de una vez</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>Que si cancelo imprimir al crear partida, me cancele todas las impresiones</t>
+  </si>
+  <si>
+    <t>Documentos de Asignacion, rutas, idioma e imprimir</t>
+  </si>
+  <si>
+    <t>Agregar y quitar cotizaciones a Partidas siempre tienen que quedar tres y el estado de SolicDetalle asociado no cambia</t>
+  </si>
+  <si>
+    <t>Agregar Inventarios a una Adquisición ya creada, Fix</t>
+  </si>
+  <si>
+    <t>Quitar Inventarios a una Adquisicion - Fix</t>
   </si>
 </sst>
 </file>
@@ -85,9 +97,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,59 +442,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
+      <c r="A5" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
+      <c r="A6" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
+      <c r="A8" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B14">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#Crear docs rendicion y partida modificar #DatosBD deserializar #Agregue plantillas al repositorio
</commit_message>
<xml_diff>
--- a/Anotaciones/Tareas.xlsx
+++ b/Anotaciones/Tareas.xlsx
@@ -410,7 +410,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,14 +454,20 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7">

</xml_diff>

<commit_message>
#Casos uso Arquitectura: - restore y backup en carpeta ya - crear log bitacora suceso en carpeta ya
</commit_message>
<xml_diff>
--- a/Anotaciones/Tareas.xlsx
+++ b/Anotaciones/Tareas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Que no me deje asociar la partida mas de una vez</t>
   </si>
@@ -56,6 +56,36 @@
   </si>
   <si>
     <t>Quitar Inventarios a una Adquisicion - Fix</t>
+  </si>
+  <si>
+    <t>Gestión de Perfiles de Usuario</t>
+  </si>
+  <si>
+    <t>Gestión de Login/Logout</t>
+  </si>
+  <si>
+    <t>Gestión de Múltiples Idiomas</t>
+  </si>
+  <si>
+    <t>Gestión de Bitácora y Control de Cambios</t>
+  </si>
+  <si>
+    <t>Gestión de Backup</t>
+  </si>
+  <si>
+    <t>Gestión de DV</t>
+  </si>
+  <si>
+    <t>Gestión de Encriptado</t>
+  </si>
+  <si>
+    <t>Casos de Prueba</t>
+  </si>
+  <si>
+    <t>Manual de Instalación</t>
+  </si>
+  <si>
+    <t>Ayuda en Línea</t>
   </si>
 </sst>
 </file>
@@ -85,7 +115,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,15 +123,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,6 +578,56 @@
         <v>5</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B10">
     <sortCondition ref="B2:B10"/>

</xml_diff>